<commit_message>
Update course info (LP AGOAPS)
</commit_message>
<xml_diff>
--- a/data/LP.xlsx
+++ b/data/LP.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/SSDS/enseignement/UFR STAPS/Direction/Outils/celcatreport/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC37968-6B09-E145-B192-7ACDEB8833A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D15863A-6085-444C-BEC6-6383BCFC807A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="19100" xr2:uid="{154AE90F-D41B-8B49-BA91-D855BEB6F170}"/>
   </bookViews>
   <sheets>
     <sheet name="LP" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -167,10 +167,10 @@
     <t>APA2551B</t>
   </si>
   <si>
-    <t>APA</t>
-  </si>
-  <si>
     <t>Groupes CM</t>
+  </si>
+  <si>
+    <t>APA2651A</t>
   </si>
 </sst>
 </file>
@@ -550,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D425352-B3D2-6642-82B3-EC9BD51219AA}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,7 +579,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>651</v>

</xml_diff>